<commit_message>
update codebook and delete never-referenced cols from data
</commit_message>
<xml_diff>
--- a/analyses/1yo_only/peril_data_deid_codebook.xlsx
+++ b/analyses/1yo_only/peril_data_deid_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ShariLiu/Dropbox (MIT)/Research/Studies/RISK/peril-infants:github/analyses/1yo_only/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907A5A91-6BCE-4646-80D0-BAD5716ADED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FD86D9-9150-204D-8D34-7C5DC9A254FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18980" yWindow="12520" windowWidth="26440" windowHeight="15440" xr2:uid="{6644F7F9-AAD9-1A43-A569-93DFC55FAB54}"/>
+    <workbookView xWindow="29000" yWindow="6640" windowWidth="26440" windowHeight="15440" xr2:uid="{6644F7F9-AAD9-1A43-A569-93DFC55FAB54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
   <si>
     <t>reliability</t>
   </si>
@@ -57,21 +57,6 @@
     <t>first_fam</t>
   </si>
   <si>
-    <t>first_test_scene</t>
-  </si>
-  <si>
-    <t>prefam_config</t>
-  </si>
-  <si>
-    <t>prefam_firstevent</t>
-  </si>
-  <si>
-    <t>prefam_1</t>
-  </si>
-  <si>
-    <t>prefam_2</t>
-  </si>
-  <si>
     <t>fam1</t>
   </si>
   <si>
@@ -108,12 +93,6 @@
     <t>sum_fam</t>
   </si>
   <si>
-    <t>avg.lower</t>
-  </si>
-  <si>
-    <t>avg.higher</t>
-  </si>
-  <si>
     <t>lower1</t>
   </si>
   <si>
@@ -126,21 +105,6 @@
     <t>higher2</t>
   </si>
   <si>
-    <t>prop.lower</t>
-  </si>
-  <si>
-    <t>prop.higher</t>
-  </si>
-  <si>
-    <t>pref.raw</t>
-  </si>
-  <si>
-    <t>pre.low</t>
-  </si>
-  <si>
-    <t>pre.high</t>
-  </si>
-  <si>
     <t>whether this participant was randomly chosen for reliability coding</t>
   </si>
   <si>
@@ -162,80 +126,185 @@
     <t>what kind of obstacle agent overcame in experiment (e.g. barrier, ramp, gap in LUTS, or depth of gap or risk in this paper)</t>
   </si>
   <si>
-    <t>which side the higher value agent was on</t>
-  </si>
-  <si>
     <t>first test event</t>
   </si>
   <si>
     <t>first familiarization event</t>
   </si>
   <si>
-    <t>for Exp 3, the left-right arrangement of the deeper and shallower trench during the first test trial</t>
-  </si>
-  <si>
-    <t>the left-right arrangement of the deeper and shallower trench during the control event</t>
-  </si>
-  <si>
-    <t>which event came first during control event</t>
-  </si>
-  <si>
-    <t>looking time during first control event</t>
-  </si>
-  <si>
-    <t>looking time during second control event</t>
-  </si>
-  <si>
-    <t>looking time during familiarization</t>
-  </si>
-  <si>
-    <t>looking time during test</t>
-  </si>
-  <si>
-    <t>average looking time during familiarization (fam 1-6)</t>
-  </si>
-  <si>
-    <t>total looking time during familiarization (fam 1-6)</t>
-  </si>
-  <si>
-    <t>average looking time towards the lower value or lower peril test event</t>
-  </si>
-  <si>
-    <t>average looking time towards the higher value or higher peril test event</t>
-  </si>
-  <si>
-    <t>looking time during the first lower value or lower peril test event</t>
-  </si>
-  <si>
-    <t>looking time during the seoncd lower value or lower peril test event</t>
-  </si>
-  <si>
-    <t>looking time during the first higher value or higher peril test event</t>
-  </si>
-  <si>
-    <t>looking time during the second higher value or higher peril test event</t>
-  </si>
-  <si>
-    <t>proportion looking towards the lower peril or lower value test event</t>
-  </si>
-  <si>
-    <t>proportion looking towards the higher peril or higher value test event</t>
-  </si>
-  <si>
-    <t>which event this participant looked longer at</t>
-  </si>
-  <si>
-    <t>looking time towards the shallower cliff during control event</t>
-  </si>
-  <si>
-    <t>looking time towards the deeper cliff during control event</t>
+    <t>explanation</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>levels</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>1, 0</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>m, f</t>
+  </si>
+  <si>
+    <t>&lt;participant id code&gt;</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>roughly 9 - 14</t>
+  </si>
+  <si>
+    <t>LUTS.Exp.&lt;x&gt; from Liu et al. 2017 Science, or MR&lt;x&gt; or RISK&lt;x&gt; for minimizing risk and inferring value from risk</t>
+  </si>
+  <si>
+    <t>Exp.&lt;1-3&gt;</t>
+  </si>
+  <si>
+    <t>Barriers, Ramps, Gap, Risk</t>
+  </si>
+  <si>
+    <t>video_quality</t>
+  </si>
+  <si>
+    <t>audio_quality</t>
+  </si>
+  <si>
+    <t>device</t>
+  </si>
+  <si>
+    <t>highchair</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>1 through 5</t>
+  </si>
+  <si>
+    <t>1 though 5</t>
+  </si>
+  <si>
+    <t>laptop, computer, ipad</t>
+  </si>
+  <si>
+    <t>for online studies, which device parents used</t>
+  </si>
+  <si>
+    <t>for online studies, parent-reported quality of stimulus 1 = very poor, 5 = very good</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t>whether this participant went through the entire study while seated in a high chair</t>
+  </si>
+  <si>
+    <t>left, right</t>
+  </si>
+  <si>
+    <t>for inferring value from X studies, which side the higher value agent was on</t>
+  </si>
+  <si>
+    <t>HV, LV, shallow, deep</t>
+  </si>
+  <si>
+    <t>HL, LH, fam1, fam2</t>
+  </si>
+  <si>
+    <t>first_test_deeper_side</t>
+  </si>
+  <si>
+    <t>control_deeper_side</t>
+  </si>
+  <si>
+    <t>control_firstevent</t>
+  </si>
+  <si>
+    <t>control_1</t>
+  </si>
+  <si>
+    <t>control_2</t>
+  </si>
+  <si>
+    <t>for min-risk studies, which side was the deeper trench on in the first test event?</t>
+  </si>
+  <si>
+    <t>for min-risk studies, which side was the deeper trench on in the first control event?</t>
+  </si>
+  <si>
+    <t>deep, shallow</t>
+  </si>
+  <si>
+    <t>for min-risk studies, for control events, which came first (deeper or shallwer)?</t>
+  </si>
+  <si>
+    <t>looking time in seconds to first control trial</t>
+  </si>
+  <si>
+    <t>range 0-60</t>
+  </si>
+  <si>
+    <t>looking time in seconds during familiarization</t>
+  </si>
+  <si>
+    <t>average looking time in seconds during familiarization (fam 1-6)</t>
+  </si>
+  <si>
+    <t>total looking time in seconds during familiarization (fam 1-6)</t>
+  </si>
+  <si>
+    <t>testavg_lower</t>
+  </si>
+  <si>
+    <t>testavg_higher</t>
+  </si>
+  <si>
+    <t>control_shallow</t>
+  </si>
+  <si>
+    <t>control_deep</t>
+  </si>
+  <si>
+    <t>average looking time in seconds during test towards the lower value or lower peril test event</t>
+  </si>
+  <si>
+    <t>average looking time in seconds during test towards the higher value or higher peril test event</t>
+  </si>
+  <si>
+    <t>looking time in seconds during the first lower value or lower peril test event</t>
+  </si>
+  <si>
+    <t>looking time in seconds during the seoncd lower value or lower peril test event</t>
+  </si>
+  <si>
+    <t>looking time in seconds during the first higher value or higher peril test event</t>
+  </si>
+  <si>
+    <t>looking time in seconds during the second higher value or higher peril test event</t>
+  </si>
+  <si>
+    <t>looking time in seconds during shallow control event</t>
+  </si>
+  <si>
+    <t>looking time in seconds during deep control event</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,6 +315,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -588,133 +663,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A8C4CA-2929-1D4E-9296-24F3C1652DE8}">
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
@@ -723,88 +699,531 @@
         <v>40</v>
       </c>
       <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
         <v>45</v>
       </c>
-      <c r="I2" t="s">
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="J2" t="s">
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="K2" t="s">
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
         <v>48</v>
       </c>
-      <c r="L2" t="s">
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>49</v>
       </c>
-      <c r="M2" t="s">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>50</v>
       </c>
-      <c r="N2" t="s">
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>51</v>
       </c>
-      <c r="O2" t="s">
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>52</v>
       </c>
-      <c r="P2" t="s">
-        <v>53</v>
-      </c>
-      <c r="V2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD2" t="s">
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="AF2" s="1" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="D13" t="s">
         <v>62</v>
       </c>
-      <c r="AH2" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
         <v>63</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>66</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>67</v>
       </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>